<commit_message>
Updated a line in the BOM descriptions
</commit_message>
<xml_diff>
--- a/hardware/retrofit controller/bills of material/TTBOM.xlsx
+++ b/hardware/retrofit controller/bills of material/TTBOM.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Walker Arce\Documents\Business\Research\UNL\StevensJeffrey\canine-dispenser\canine_dispenser\canine_dispenser\hardware\BOM\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub Repos\canine_treat_dispenser\hardware\retrofit controller\bills of material\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C47FE048-4C25-474A-934B-EFE4B290F223}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32E91C7E-1929-4F0C-A1B0-2A4483169627}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{848C24C6-6C92-4413-9B7A-75618992047C}"/>
   </bookViews>
@@ -71,9 +71,6 @@
     <t>BAS16J</t>
   </si>
   <si>
-    <t>Weather Sensor Diodes</t>
-  </si>
-  <si>
     <t xml:space="preserve">1727-6169-1-ND	</t>
   </si>
   <si>
@@ -417,6 +414,9 @@
   </si>
   <si>
     <t xml:space="preserve">CF14JT1K00CT-ND </t>
+  </si>
+  <si>
+    <t>Reset Circuit Bias</t>
   </si>
 </sst>
 </file>
@@ -900,8 +900,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{593F0E4E-37F7-4819-A383-F6E78936B304}">
   <dimension ref="A1:T32"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="D4" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="I13" sqref="I13"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -931,7 +931,7 @@
   <sheetData>
     <row r="1" spans="1:20" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="29" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B1" s="29"/>
       <c r="C1" s="29"/>
@@ -940,13 +940,13 @@
       <c r="F1" s="29"/>
       <c r="G1" s="29"/>
       <c r="I1" s="29" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="J1" s="29"/>
       <c r="K1" s="29"/>
       <c r="L1" s="29"/>
       <c r="N1" s="29" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="O1" s="29"/>
       <c r="P1" s="29"/>
@@ -975,7 +975,7 @@
         <v>7</v>
       </c>
       <c r="G2" s="15" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="I2" s="13" t="s">
         <v>0</v>
@@ -1008,21 +1008,21 @@
         <v>7</v>
       </c>
       <c r="T2" s="15" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="3" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C3" s="4" t="s">
         <v>5</v>
       </c>
       <c r="D3" s="5" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E3" s="6">
         <v>1</v>
@@ -1035,10 +1035,10 @@
         <v>2.92</v>
       </c>
       <c r="I3" s="19" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="J3" s="19" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="K3" s="20">
         <v>1</v>
@@ -1047,16 +1047,16 @@
         <v>59.95</v>
       </c>
       <c r="N3" s="19" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="O3" s="19" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="P3" s="19" t="s">
         <v>5</v>
       </c>
       <c r="Q3" s="27" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="R3" s="20">
         <v>1</v>
@@ -1071,16 +1071,16 @@
     </row>
     <row r="4" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A4" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="B4" s="8" t="s">
         <v>51</v>
       </c>
-      <c r="B4" s="8" t="s">
+      <c r="C4" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="D4" s="8" t="s">
         <v>52</v>
-      </c>
-      <c r="C4" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="D4" s="8" t="s">
-        <v>53</v>
       </c>
       <c r="E4" s="3">
         <v>1</v>
@@ -1093,10 +1093,10 @@
         <v>1.95</v>
       </c>
       <c r="I4" s="8" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="J4" s="8" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="K4" s="3">
         <v>1</v>
@@ -1105,16 +1105,16 @@
         <v>6.99</v>
       </c>
       <c r="N4" s="8" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="O4" s="8" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="P4" s="8" t="s">
         <v>5</v>
       </c>
       <c r="Q4" s="23" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="R4" s="3">
         <v>1</v>
@@ -1129,16 +1129,16 @@
     </row>
     <row r="5" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A5" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="B5" s="8" t="s">
         <v>54</v>
       </c>
-      <c r="B5" s="8" t="s">
+      <c r="C5" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="D5" s="8" t="s">
         <v>55</v>
-      </c>
-      <c r="C5" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="D5" s="8" t="s">
-        <v>56</v>
       </c>
       <c r="E5" s="3">
         <v>1</v>
@@ -1151,10 +1151,10 @@
         <v>1.64</v>
       </c>
       <c r="I5" s="8" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="J5" s="8" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="K5" s="3">
         <v>1</v>
@@ -1163,13 +1163,13 @@
         <v>8</v>
       </c>
       <c r="N5" s="8" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="O5" s="8" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="P5" s="8" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="Q5" s="26">
         <v>2117</v>
@@ -1187,16 +1187,16 @@
     </row>
     <row r="6" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="B6" s="4" t="s">
         <v>74</v>
       </c>
-      <c r="B6" s="4" t="s">
+      <c r="C6" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D6" s="5" t="s">
         <v>75</v>
-      </c>
-      <c r="C6" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="D6" s="5" t="s">
-        <v>76</v>
       </c>
       <c r="E6" s="6">
         <v>1</v>
@@ -1209,10 +1209,10 @@
         <v>0.49</v>
       </c>
       <c r="I6" s="8" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="J6" s="8" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="K6" s="3">
         <v>1</v>
@@ -1221,16 +1221,16 @@
         <v>8.99</v>
       </c>
       <c r="N6" s="8" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="O6" s="8" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="P6" s="8" t="s">
         <v>5</v>
       </c>
       <c r="Q6" s="23" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="R6" s="3">
         <v>3</v>
@@ -1245,16 +1245,16 @@
     </row>
     <row r="7" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A7" s="8" t="s">
+        <v>58</v>
+      </c>
+      <c r="B7" s="8" t="s">
         <v>59</v>
       </c>
-      <c r="B7" s="8" t="s">
+      <c r="C7" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="D7" s="8" t="s">
         <v>60</v>
-      </c>
-      <c r="C7" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="D7" s="8" t="s">
-        <v>61</v>
       </c>
       <c r="E7" s="3">
         <v>1</v>
@@ -1267,10 +1267,10 @@
         <v>1.1100000000000001</v>
       </c>
       <c r="I7" s="8" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="J7" s="8" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="K7" s="3">
         <v>1</v>
@@ -1279,16 +1279,16 @@
         <v>1.59</v>
       </c>
       <c r="N7" s="8" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="O7" s="8" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="P7" s="8" t="s">
         <v>5</v>
       </c>
       <c r="Q7" s="23" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="R7" s="3">
         <v>1</v>
@@ -1303,16 +1303,16 @@
     </row>
     <row r="8" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A8" s="8" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B8" s="8" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C8" s="8" t="s">
         <v>5</v>
       </c>
       <c r="D8" s="8" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="E8" s="3">
         <v>3</v>
@@ -1325,10 +1325,10 @@
         <v>3.09</v>
       </c>
       <c r="I8" s="8" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="J8" s="8" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="K8" s="3">
         <v>1</v>
@@ -1337,16 +1337,16 @@
         <v>5.41</v>
       </c>
       <c r="N8" s="8" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="O8" s="8" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="P8" s="8" t="s">
         <v>5</v>
       </c>
       <c r="Q8" s="23" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="R8" s="3">
         <v>4</v>
@@ -1361,16 +1361,16 @@
     </row>
     <row r="9" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B9" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="B9" s="4" t="s">
+      <c r="C9" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D9" s="5" t="s">
         <v>15</v>
-      </c>
-      <c r="C9" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="D9" s="5" t="s">
-        <v>16</v>
       </c>
       <c r="E9" s="6">
         <v>1</v>
@@ -1383,10 +1383,10 @@
         <v>0.69</v>
       </c>
       <c r="I9" s="16" t="s">
+        <v>101</v>
+      </c>
+      <c r="J9" s="16" t="s">
         <v>102</v>
-      </c>
-      <c r="J9" s="16" t="s">
-        <v>103</v>
       </c>
       <c r="K9" s="17">
         <v>1</v>
@@ -1395,16 +1395,16 @@
         <v>1.95</v>
       </c>
       <c r="N9" s="8" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="O9" s="8" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="P9" s="8" t="s">
         <v>5</v>
       </c>
       <c r="Q9" s="23" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="R9" s="3">
         <v>2</v>
@@ -1419,16 +1419,16 @@
     </row>
     <row r="10" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="B10" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="B10" s="4" t="s">
+      <c r="C10" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D10" s="4" t="s">
         <v>35</v>
-      </c>
-      <c r="C10" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="D10" s="4" t="s">
-        <v>36</v>
       </c>
       <c r="E10" s="6">
         <v>1</v>
@@ -1441,16 +1441,16 @@
         <v>0.1</v>
       </c>
       <c r="N10" s="8" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="O10" s="8" t="s">
+        <v>121</v>
+      </c>
+      <c r="P10" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="Q10" s="23" t="s">
         <v>122</v>
-      </c>
-      <c r="P10" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="Q10" s="23" t="s">
-        <v>123</v>
       </c>
       <c r="R10" s="3">
         <v>2</v>
@@ -1465,16 +1465,16 @@
     </row>
     <row r="11" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="B11" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="B11" s="4" t="s">
+      <c r="C11" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D11" s="5" t="s">
         <v>39</v>
-      </c>
-      <c r="C11" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="D11" s="5" t="s">
-        <v>40</v>
       </c>
       <c r="E11" s="6">
         <v>1</v>
@@ -1491,16 +1491,16 @@
         <v>92.88</v>
       </c>
       <c r="N11" s="16" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="O11" s="16" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="P11" s="16" t="s">
         <v>5</v>
       </c>
       <c r="Q11" s="28" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="R11" s="17">
         <v>1</v>
@@ -1515,16 +1515,16 @@
     </row>
     <row r="12" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="B12" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="B12" s="4" t="s">
+      <c r="C12" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D12" s="5" t="s">
         <v>23</v>
-      </c>
-      <c r="C12" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="D12" s="5" t="s">
-        <v>24</v>
       </c>
       <c r="E12" s="6">
         <v>4</v>
@@ -1547,16 +1547,16 @@
     </row>
     <row r="13" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="B13" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="B13" s="4" t="s">
+      <c r="C13" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D13" s="5" t="s">
         <v>19</v>
-      </c>
-      <c r="C13" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="D13" s="5" t="s">
-        <v>20</v>
       </c>
       <c r="E13" s="6">
         <v>1</v>
@@ -1571,16 +1571,16 @@
     </row>
     <row r="14" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A14" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="B14" s="8" t="s">
         <v>41</v>
       </c>
-      <c r="B14" s="8" t="s">
+      <c r="C14" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="D14" s="8" t="s">
         <v>42</v>
-      </c>
-      <c r="C14" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="D14" s="8" t="s">
-        <v>43</v>
       </c>
       <c r="E14" s="3">
         <v>1</v>
@@ -1598,13 +1598,13 @@
         <v>11</v>
       </c>
       <c r="B15" s="4" t="s">
+        <v>127</v>
+      </c>
+      <c r="C15" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D15" s="5" t="s">
         <v>12</v>
-      </c>
-      <c r="C15" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="D15" s="5" t="s">
-        <v>13</v>
       </c>
       <c r="E15" s="6">
         <v>1</v>
@@ -1619,16 +1619,16 @@
     </row>
     <row r="16" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A16" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B16" s="9" t="s">
+        <v>56</v>
+      </c>
+      <c r="C16" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D16" s="10" t="s">
         <v>57</v>
-      </c>
-      <c r="C16" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="D16" s="10" t="s">
-        <v>58</v>
       </c>
       <c r="E16" s="6">
         <v>3</v>
@@ -1643,16 +1643,16 @@
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="B17" s="8" t="s">
         <v>44</v>
       </c>
-      <c r="B17" s="8" t="s">
+      <c r="C17" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="D17" s="8" t="s">
         <v>45</v>
-      </c>
-      <c r="C17" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="D17" s="8" t="s">
-        <v>46</v>
       </c>
       <c r="E17" s="3">
         <v>1</v>
@@ -1667,16 +1667,16 @@
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="B18" s="8" t="s">
         <v>47</v>
       </c>
-      <c r="B18" s="8" t="s">
+      <c r="C18" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="D18" s="8" t="s">
         <v>48</v>
-      </c>
-      <c r="C18" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="D18" s="8" t="s">
-        <v>49</v>
       </c>
       <c r="E18" s="3">
         <v>1</v>
@@ -1691,16 +1691,16 @@
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" s="8" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B19" s="8" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C19" s="8" t="s">
         <v>5</v>
       </c>
       <c r="D19" s="8" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E19" s="3">
         <v>1</v>
@@ -1715,16 +1715,16 @@
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" s="4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C20" s="4" t="s">
         <v>5</v>
       </c>
       <c r="D20" s="5" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="E20" s="6">
         <v>9</v>
@@ -1739,16 +1739,16 @@
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="B21" s="11" t="s">
         <v>69</v>
       </c>
-      <c r="B21" s="11" t="s">
+      <c r="C21" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D21" s="4" t="s">
         <v>70</v>
-      </c>
-      <c r="C21" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="D21" s="4" t="s">
-        <v>71</v>
       </c>
       <c r="E21" s="6">
         <v>3</v>
@@ -1763,16 +1763,16 @@
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" s="8" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B22" s="8" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C22" s="8" t="s">
         <v>5</v>
       </c>
       <c r="D22" s="8" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="E22" s="3">
         <v>1</v>
@@ -1787,16 +1787,16 @@
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" s="8" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B23" s="8" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C23" s="8" t="s">
         <v>5</v>
       </c>
       <c r="D23" s="8" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="E23" s="3">
         <v>1</v>
@@ -1811,16 +1811,16 @@
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" s="8" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B24" s="8" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C24" s="8" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D24" s="8" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="E24" s="3">
         <v>1</v>
@@ -1835,16 +1835,16 @@
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" s="8" t="s">
+        <v>65</v>
+      </c>
+      <c r="B25" s="8" t="s">
         <v>66</v>
       </c>
-      <c r="B25" s="8" t="s">
-        <v>67</v>
-      </c>
       <c r="C25" s="8" t="s">
         <v>5</v>
       </c>
       <c r="D25" s="8" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="E25" s="3">
         <v>1</v>
@@ -1859,16 +1859,16 @@
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" s="8" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B26" s="8" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C26" s="8" t="s">
         <v>5</v>
       </c>
       <c r="D26" s="8" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="E26" s="3">
         <v>1</v>
@@ -1883,16 +1883,16 @@
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="B27" s="4" t="s">
         <v>26</v>
-      </c>
-      <c r="B27" s="4" t="s">
-        <v>27</v>
       </c>
       <c r="C27" s="4" t="s">
         <v>6</v>
       </c>
       <c r="D27" s="12" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E27" s="6">
         <v>2</v>
@@ -1907,16 +1907,16 @@
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="B28" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="B28" s="4" t="s">
+      <c r="C28" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D28" s="5" t="s">
         <v>31</v>
-      </c>
-      <c r="C28" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="D28" s="5" t="s">
-        <v>32</v>
       </c>
       <c r="E28" s="6">
         <v>7</v>
@@ -1955,16 +1955,16 @@
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" s="8" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B30" s="8" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C30" s="8" t="s">
         <v>5</v>
       </c>
       <c r="D30" s="8" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="E30" s="3">
         <v>1</v>
@@ -1979,16 +1979,16 @@
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" s="16" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B31" s="16" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C31" s="16" t="s">
         <v>5</v>
       </c>
       <c r="D31" s="16" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="E31" s="17">
         <v>4</v>

</xml_diff>